<commit_message>
Front || Cambios nueva solicitud cliente
</commit_message>
<xml_diff>
--- a/NormalizacionBD_ICUAP.xlsx
+++ b/NormalizacionBD_ICUAP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarki\Documents\GitHub\ICUAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E81D563-F505-EE41-A3A4-33C8C6E5D397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F044730F-2141-4950-8A8E-D729CCF57835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3D578A57-378C-4291-A136-BCC763F665B7}"/>
   </bookViews>
@@ -282,6 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -291,16 +292,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,27 +621,27 @@
       <selection activeCell="B10" sqref="B10:G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.23828125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5078125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -654,10 +654,10 @@
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
@@ -666,7 +666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -677,7 +677,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -688,7 +688,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -699,7 +699,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -710,24 +710,24 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
@@ -738,7 +738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -746,7 +746,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -754,7 +754,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -762,7 +762,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -770,23 +770,23 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="5" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="6"/>
+      <c r="D19" s="7"/>
       <c r="E19" s="1" t="s">
         <v>15</v>
       </c>
@@ -794,71 +794,71 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="5" t="s">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="5" t="s">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5" t="s">
+      <c r="C27" s="6"/>
+      <c r="D27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -888,31 +888,31 @@
       <selection activeCell="J15" sqref="J15:M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.9140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.046875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.23828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="J5" s="5" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="J5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
@@ -928,10 +928,10 @@
       <c r="J6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="7"/>
       <c r="M6" s="1" t="s">
         <v>10</v>
       </c>
@@ -942,7 +942,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -954,7 +954,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -966,7 +966,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -978,7 +978,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -990,45 +990,45 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="5" t="s">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="J15" s="5" t="s">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="J15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5" t="s">
+      <c r="K16" s="6"/>
+      <c r="L16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M16" s="5"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1039,7 +1039,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1050,7 +1050,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1061,7 +1061,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1072,7 +1072,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1102,32 +1102,32 @@
       <selection activeCell="F23" sqref="F23:G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.9140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.64453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5078125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="H4" s="5" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="H4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="L4" s="5" t="s">
+      <c r="I4" s="6"/>
+      <c r="L4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1163,7 +1163,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1173,7 +1173,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1183,7 +1183,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1193,38 +1193,38 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="H13" s="7" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="H13" s="8" t="s">
         <v>8</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="8"/>
-      <c r="O13" s="7" t="s">
+      <c r="M13" s="10"/>
+      <c r="O13" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="1" t="s">
         <v>27</v>
       </c>
@@ -1234,10 +1234,10 @@
       <c r="I14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="K14" s="7"/>
       <c r="L14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1251,85 +1251,85 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="10"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="10"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="10"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="10"/>
       <c r="F18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="10"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B23" s="7" t="s">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="9"/>
-      <c r="D23" s="8"/>
-      <c r="F23" s="5" t="s">
+      <c r="D23" s="10"/>
+      <c r="F23" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1357,7 +1357,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1368,18 +1368,26 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="H13:M13"/>
@@ -1391,14 +1399,6 @@
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="J18:K18"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1408,36 +1408,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB86361F-4B1F-4000-BF25-634B2C985BA4}">
   <dimension ref="C4:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12.9140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.64453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C4" s="5" t="s">
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="K4" s="5" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="K4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="O4" s="5" t="s">
+      <c r="L4" s="6"/>
+      <c r="O4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="5"/>
-    </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="P4" s="6"/>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>40</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1481,7 +1481,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1493,7 +1493,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1505,7 +1505,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1517,41 +1517,41 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C14" s="5" t="s">
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="K14" s="5" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="K14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="U14" s="7" t="s">
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="U14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="V14" s="8"/>
-    </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="V14" s="10"/>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1564,10 +1564,10 @@
       <c r="L15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M15" s="6" t="s">
+      <c r="M15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="N15" s="6"/>
+      <c r="N15" s="7"/>
       <c r="O15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1587,17 +1587,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
@@ -1605,17 +1605,17 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
     </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -1623,17 +1623,17 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -1641,17 +1641,17 @@
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
     </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -1659,32 +1659,32 @@
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
     </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C24" s="5" t="s">
+    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="I24" s="5" t="s">
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="I24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="5"/>
-      <c r="M24" s="10" t="s">
+      <c r="J24" s="6"/>
+      <c r="M24" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-    </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+    </row>
+    <row r="25" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>29</v>
       </c>
@@ -1703,17 +1703,17 @@
       <c r="J25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M25" s="11" t="s">
+      <c r="M25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N25" s="11" t="s">
+      <c r="N25" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="O25" s="11" t="s">
+      <c r="O25" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1724,11 +1724,11 @@
       <c r="J26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11"/>
-    </row>
-    <row r="27" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1739,41 +1739,30 @@
       <c r="J27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-    </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-    </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.2">
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="K14:R14"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C14:H14"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="C24:F24"/>
     <mergeCell ref="M16:N16"/>
@@ -1783,6 +1772,17 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M24:O24"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="K14:R14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>